<commit_message>
Realizacion de backup, serializacion,bitacora de eventos.
</commit_message>
<xml_diff>
--- a/Informe de facturas.xlsx
+++ b/Informe de facturas.xlsx
@@ -185,8 +185,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G18" totalsRowShown="0">
-  <x:autoFilter ref="A1:G18"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G19" totalsRowShown="0">
+  <x:autoFilter ref="A1:G19"/>
   <x:tableColumns count="7">
     <x:tableColumn id="1" name="Fecha" dataDxfId="0"/>
     <x:tableColumn id="2" name="Monto_Total"/>
@@ -488,7 +488,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:G18"/>
+  <x:dimension ref="A1:G19"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -906,6 +906,29 @@
       </x:c>
       <x:c r="G18" s="0" t="s">
         <x:v>31</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:7">
+      <x:c r="A19" s="1">
+        <x:v>45529</x:v>
+      </x:c>
+      <x:c r="B19" s="0">
+        <x:v>120000</x:v>
+      </x:c>
+      <x:c r="C19" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D19" s="0">
+        <x:v>45225577</x:v>
+      </x:c>
+      <x:c r="E19" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="F19" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="G19" s="0" t="s">
+        <x:v>28</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>